<commit_message>
features:   ＊chip analysis: crawl the foreign & sic & dealer's trading history   ＊batch runner: ignore the error as the market not open
</commit_message>
<xml_diff>
--- a/database/d-developing/法人進出明細.xlsx
+++ b/database/d-developing/法人進出明細.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="0" windowWidth="22740" windowHeight="15020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2860" yWindow="0" windowWidth="22740" windowHeight="15020" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="tracking" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,148 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
-  <si>
-    <t>議題層面</t>
-  </si>
-  <si>
-    <t>需求控管</t>
-  </si>
-  <si>
-    <t>效益：降低因需求模糊而衍生的設計變更，降低需求爭議及因為爭議而致無償修改</t>
-  </si>
-  <si>
-    <t>行動方案 (*：今年)與效益</t>
-  </si>
-  <si>
-    <t>測試有效性</t>
-  </si>
-  <si>
-    <t>•測試實務方法建立 (測試環境、資料準備)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">•測試方法導入 (實作與輔導) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">•產品核心功能自動化/迴歸測試 </t>
-  </si>
-  <si>
-    <t>•程序準則：測試計畫、整合策略</t>
-  </si>
-  <si>
-    <t>水平分工造成工作銜接的困難與重工(coding pool)</t>
-  </si>
-  <si>
-    <t>•程序準則：系統分析產出標準與應用</t>
-  </si>
-  <si>
-    <t>•開發過程 vs. 增修/ 維護</t>
-  </si>
-  <si>
-    <t>•修訂程序：開發啟動會議 (開發說明會)</t>
-  </si>
-  <si>
-    <t>•修訂程序：共用設計/共通規範樣板建立</t>
-  </si>
-  <si>
-    <t>進展</t>
-  </si>
-  <si>
-    <t>成效</t>
-  </si>
-  <si>
-    <t>瓶頸</t>
-  </si>
-  <si>
-    <t>需要支援</t>
-  </si>
-  <si>
-    <t>預期效益</t>
-  </si>
-  <si>
-    <t>版本控管方法</t>
-  </si>
-  <si>
-    <t>共通性功能需求經驗分享與再利用</t>
-  </si>
-  <si>
-    <t>複雜技術解決能量養成</t>
-  </si>
-  <si>
-    <t>•版本控制與發行管理方法及能力養成</t>
-  </si>
-  <si>
-    <t>•程序修訂：擬定建構項目的必要性</t>
-  </si>
-  <si>
-    <t>•程式、資料庫、系統參數/設定</t>
-  </si>
-  <si>
-    <t>•提昇軟體發行品質</t>
-  </si>
-  <si>
-    <t>•縮短併版時間</t>
-  </si>
-  <si>
-    <t>•建立分享與易於搜尋機制  (KM + GIT/SVN)</t>
-  </si>
-  <si>
-    <t>•程序修訂：加入「共用或關鍵性功能分析與產出作業」，列入架構設計審查</t>
-  </si>
-  <si>
-    <t>•降低重複開發成本</t>
-  </si>
-  <si>
-    <t>•落實BG技術團隊建立(救火隊)</t>
-  </si>
-  <si>
-    <t>•建立技術支援模式 （TDS_SUPPORT）</t>
-  </si>
-  <si>
-    <t>•定期高手間的經驗分享與傳承（每月）</t>
-  </si>
-  <si>
-    <t>•縮短問題解決時間與成本</t>
-  </si>
-  <si>
-    <t>•縮短流程/功能測試（SA）時間與成本•降低複雜功能（計算/報表）重工率</t>
-  </si>
-  <si>
-    <t>•縮短規格開立（SA）時間與成本•提昇系統分析與操作的一致性</t>
-  </si>
-  <si>
-    <t>1.Corp提供使用情境式訓練 (PMIS及JIRA)</t>
-  </si>
-  <si>
-    <t>2.BG 定義 BG/BU 共用 WBS 範本</t>
-  </si>
-  <si>
-    <t>3.里程碑管控：需求SA /架構設計 review</t>
-  </si>
-  <si>
-    <t>4.加強風險專案監控與共商因應對策</t>
-  </si>
-  <si>
-    <t>5.專案結案 AAR</t>
-  </si>
-  <si>
-    <t>效益：節省PM時間、共享 WBS Template、</t>
-  </si>
-  <si>
-    <t>提升對專案的管控方式與能力、CPI/SPI 反映真實情況</t>
-  </si>
-  <si>
-    <t>1.需求與分析的審查</t>
-  </si>
-  <si>
-    <t>2.程序：系統需求規格書大綱、內容範例</t>
-  </si>
-  <si>
-    <t>3.中期計畫(訓練與程序)：如何釐清、需求導出、範圍、priority、協商與管理等</t>
-  </si>
-  <si>
-    <t>專案控管及工具整合、專案進度透通</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Code</t>
   </si>
@@ -323,7 +181,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -347,12 +205,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Heiti TC Light"/>
-      <charset val="136"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -362,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -370,58 +222,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -476,39 +276,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="51">
@@ -891,382 +660,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="19.83203125" customWidth="1"/>
-    <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="41.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="26">
-      <c r="A2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="8"/>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="8"/>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="26">
-      <c r="A6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="8"/>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="8"/>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="7"/>
-      <c r="B11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="7"/>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" ht="26">
-      <c r="A14" s="6"/>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="7"/>
-      <c r="B16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="7"/>
-      <c r="B17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="4"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1">
-      <c r="A19" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" ht="27">
-      <c r="A20" s="8"/>
-      <c r="B20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8"/>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="8"/>
-      <c r="B22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="8"/>
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="27">
-      <c r="A24" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="10"/>
-      <c r="B25" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="26">
-      <c r="A26" s="10"/>
-      <c r="B26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="11"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="A24:A27"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1277,52 +670,52 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -1330,15 +723,15 @@
         <v>3553</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="12">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1">
         <v>2000</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="1">
         <v>2000</v>
       </c>
       <c r="F2">
@@ -1371,7 +764,7 @@
       <c r="O2">
         <v>0</v>
       </c>
-      <c r="P2" s="12">
+      <c r="P2" s="1">
         <v>2000</v>
       </c>
     </row>
@@ -1380,15 +773,15 @@
         <v>5508</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="12">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1">
         <v>8000</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="1">
         <v>7000</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="1">
         <v>1000</v>
       </c>
       <c r="F3">
@@ -1421,7 +814,7 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3" s="12">
+      <c r="P3" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -1430,24 +823,24 @@
         <v>2726</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="12">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1">
         <v>4000</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="1">
         <v>6000</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="1">
         <v>-2000</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="1">
         <v>9000</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="1">
         <v>9000</v>
       </c>
       <c r="I4">
@@ -1471,7 +864,7 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="1">
         <v>7000</v>
       </c>
     </row>
@@ -1480,15 +873,15 @@
         <v>6023</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="12">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1">
         <v>6000</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="1">
         <v>37000</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="1">
         <v>-31000</v>
       </c>
       <c r="F5">
@@ -1521,7 +914,7 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5" s="12">
+      <c r="P5" s="1">
         <v>-31000</v>
       </c>
     </row>
@@ -1530,15 +923,15 @@
         <v>5474</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="12">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1">
         <v>26000</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="1">
         <v>40000</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="1">
         <v>-14000</v>
       </c>
       <c r="F6">
@@ -1571,7 +964,7 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6" s="12">
+      <c r="P6" s="1">
         <v>-14000</v>
       </c>
     </row>
@@ -1580,15 +973,15 @@
         <v>6261</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
-      </c>
-      <c r="C7" s="12">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
         <v>89000</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="1">
         <v>7000</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="1">
         <v>82000</v>
       </c>
       <c r="F7">
@@ -1600,16 +993,16 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I7" s="1">
         <v>-9000</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="1">
         <v>9000</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="1">
         <v>-9000</v>
       </c>
       <c r="M7">
@@ -1621,7 +1014,7 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="1">
         <v>73000</v>
       </c>
     </row>
@@ -1630,15 +1023,15 @@
         <v>4711</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="12">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
         <v>9000</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="1">
         <v>9000</v>
       </c>
       <c r="F8">
@@ -1650,16 +1043,16 @@
       <c r="H8">
         <v>0</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="1">
         <v>17000</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="1">
         <v>17000</v>
       </c>
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="1">
         <v>17000</v>
       </c>
       <c r="M8">
@@ -1671,7 +1064,7 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8" s="12">
+      <c r="P8" s="1">
         <v>26000</v>
       </c>
     </row>
@@ -1680,15 +1073,15 @@
         <v>6220</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="12">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
         <v>248000</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="1">
         <v>124000</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="1">
         <v>124000</v>
       </c>
       <c r="F9">
@@ -1700,16 +1093,16 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="1">
         <v>-316000</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="1">
         <v>316000</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="1">
         <v>-316000</v>
       </c>
       <c r="M9">
@@ -1721,7 +1114,7 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9" s="12">
+      <c r="P9" s="1">
         <v>-192000</v>
       </c>
     </row>
@@ -1730,7 +1123,7 @@
         <v>6201</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1750,7 +1143,7 @@
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="I10" s="12">
+      <c r="I10" s="1">
         <v>-4000</v>
       </c>
       <c r="J10">
@@ -1765,13 +1158,13 @@
       <c r="M10">
         <v>0</v>
       </c>
-      <c r="N10" s="12">
+      <c r="N10" s="1">
         <v>4000</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="1">
         <v>-4000</v>
       </c>
-      <c r="P10" s="12">
+      <c r="P10" s="1">
         <v>-4000</v>
       </c>
     </row>
@@ -1780,15 +1173,15 @@
         <v>8942</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="12">
+        <v>25</v>
+      </c>
+      <c r="C11" s="1">
         <v>85000</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="1">
         <v>10000</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="1">
         <v>75000</v>
       </c>
       <c r="F11">
@@ -1800,7 +1193,7 @@
       <c r="H11">
         <v>0</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="1">
         <v>8000</v>
       </c>
       <c r="J11">
@@ -1812,16 +1205,16 @@
       <c r="L11">
         <v>0</v>
       </c>
-      <c r="M11" s="12">
+      <c r="M11" s="1">
         <v>10000</v>
       </c>
-      <c r="N11" s="12">
+      <c r="N11" s="1">
         <v>2000</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="1">
         <v>8000</v>
       </c>
-      <c r="P11" s="12">
+      <c r="P11" s="1">
         <v>83000</v>
       </c>
     </row>
@@ -1897,52 +1290,52 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>77</v>
+        <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="G16" t="s">
-        <v>79</v>
+        <v>32</v>
       </c>
       <c r="H16" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="J16" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="K16" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="M16" t="s">
-        <v>85</v>
+        <v>38</v>
       </c>
       <c r="N16" t="s">
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="O16" t="s">
-        <v>87</v>
+        <v>40</v>
       </c>
       <c r="P16" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1950,15 +1343,15 @@
         <v>1258</v>
       </c>
       <c r="B17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="12">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1">
         <v>1000</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="1">
         <v>2000</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="1">
         <v>-1000</v>
       </c>
       <c r="F17">
@@ -1991,7 +1384,7 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17" s="12">
+      <c r="P17" s="1">
         <v>-1000</v>
       </c>
     </row>
@@ -2000,15 +1393,15 @@
         <v>1264</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="1">
         <v>1000</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="1">
         <v>-1000</v>
       </c>
       <c r="F18">
@@ -2041,7 +1434,7 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18" s="12">
+      <c r="P18" s="1">
         <v>-1000</v>
       </c>
     </row>
@@ -2050,15 +1443,15 @@
         <v>1565</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="12">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1">
         <v>23000</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="1">
         <v>9000</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="1">
         <v>14000</v>
       </c>
       <c r="F19">
@@ -2070,28 +1463,28 @@
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="12">
+      <c r="I19" s="1">
         <v>-10000</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="1">
         <v>4000</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="1">
         <v>-4000</v>
       </c>
       <c r="M19">
         <v>0</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="1">
         <v>6000</v>
       </c>
-      <c r="O19" s="12">
+      <c r="O19" s="1">
         <v>-6000</v>
       </c>
-      <c r="P19" s="12">
+      <c r="P19" s="1">
         <v>4000</v>
       </c>
     </row>
@@ -2100,15 +1493,15 @@
         <v>1566</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="12">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1">
         <v>1000</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="1">
         <v>1000</v>
       </c>
       <c r="F20">
@@ -2141,7 +1534,7 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20" s="12">
+      <c r="P20" s="1">
         <v>1000</v>
       </c>
     </row>
@@ -2150,15 +1543,15 @@
         <v>1569</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="12">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1">
         <v>68000</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="1">
         <v>308000</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="1">
         <v>-240000</v>
       </c>
       <c r="F21">
@@ -2191,7 +1584,7 @@
       <c r="O21">
         <v>0</v>
       </c>
-      <c r="P21" s="12">
+      <c r="P21" s="1">
         <v>-240000</v>
       </c>
     </row>
@@ -2200,7 +1593,7 @@
         <v>1570</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2220,16 +1613,16 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22" s="12">
+      <c r="I22" s="1">
         <v>6000</v>
       </c>
-      <c r="J22" s="12">
+      <c r="J22" s="1">
         <v>6000</v>
       </c>
       <c r="K22">
         <v>0</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="1">
         <v>6000</v>
       </c>
       <c r="M22">
@@ -2241,7 +1634,7 @@
       <c r="O22">
         <v>0</v>
       </c>
-      <c r="P22" s="12">
+      <c r="P22" s="1">
         <v>6000</v>
       </c>
     </row>
@@ -2250,24 +1643,24 @@
         <v>1580</v>
       </c>
       <c r="B23" t="s">
-        <v>94</v>
-      </c>
-      <c r="C23" s="12">
+        <v>47</v>
+      </c>
+      <c r="C23" s="1">
         <v>41000</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="1">
         <v>10000</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="1">
         <v>31000</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="1">
         <v>24000</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H23" s="1">
         <v>24000</v>
       </c>
       <c r="I23">
@@ -2291,7 +1684,7 @@
       <c r="O23">
         <v>0</v>
       </c>
-      <c r="P23" s="12">
+      <c r="P23" s="1">
         <v>55000</v>
       </c>
     </row>
@@ -2300,15 +1693,15 @@
         <v>1584</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C24" s="12">
+        <v>48</v>
+      </c>
+      <c r="C24" s="1">
         <v>6000</v>
       </c>
-      <c r="D24" s="12">
+      <c r="D24" s="1">
         <v>8000</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="1">
         <v>-2000</v>
       </c>
       <c r="F24">
@@ -2341,7 +1734,7 @@
       <c r="O24">
         <v>0</v>
       </c>
-      <c r="P24" s="12">
+      <c r="P24" s="1">
         <v>-2000</v>
       </c>
     </row>
@@ -2350,15 +1743,15 @@
         <v>1586</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="12">
+        <v>49</v>
+      </c>
+      <c r="C25" s="1">
         <v>28000</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25" s="1">
         <v>3000</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="1">
         <v>25000</v>
       </c>
       <c r="F25">
@@ -2391,7 +1784,7 @@
       <c r="O25">
         <v>0</v>
       </c>
-      <c r="P25" s="12">
+      <c r="P25" s="1">
         <v>25000</v>
       </c>
     </row>
@@ -2400,15 +1793,15 @@
         <v>1591</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="1">
         <v>5000</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="1">
         <v>-5000</v>
       </c>
       <c r="F26">
@@ -2420,16 +1813,16 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26" s="12">
+      <c r="I26" s="1">
         <v>-6000</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
-      <c r="K26" s="12">
+      <c r="K26" s="1">
         <v>6000</v>
       </c>
-      <c r="L26" s="12">
+      <c r="L26" s="1">
         <v>-6000</v>
       </c>
       <c r="M26">
@@ -2441,7 +1834,7 @@
       <c r="O26">
         <v>0</v>
       </c>
-      <c r="P26" s="12">
+      <c r="P26" s="1">
         <v>-11000</v>
       </c>
     </row>

</xml_diff>